<commit_message>
fix eu tabelle for faktenblatt and other small things
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2020-12-13.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2020-12-13.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="211">
   <si>
     <t xml:space="preserve">Testungen</t>
   </si>
@@ -198,27 +198,6 @@
     <t xml:space="preserve"> 6,0 %</t>
   </si>
   <si>
-    <t xml:space="preserve">Regionen mit 7-TI bei Über-80-Jährigen:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">362</t>
-  </si>
-  <si>
-    <t xml:space="preserve">382</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5,5 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">350</t>
-  </si>
-  <si>
-    <t xml:space="preserve">376</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,4 %</t>
-  </si>
-  <si>
     <t xml:space="preserve">Intensivbetten</t>
   </si>
   <si>
@@ -237,11 +216,11 @@
     <t xml:space="preserve">Belegung durch Patient*innen mit COVID-19</t>
   </si>
   <si>
-    <t xml:space="preserve">15 %, 
+    <t xml:space="preserve">15 %
 4108</t>
   </si>
   <si>
-    <t xml:space="preserve">17 %, 
+    <t xml:space="preserve">17 %
 4552</t>
   </si>
   <si>
@@ -251,11 +230,11 @@
     <t xml:space="preserve">Freie Intensivbetten</t>
   </si>
   <si>
-    <t xml:space="preserve">20 %, 
+    <t xml:space="preserve">20 %
 5539</t>
   </si>
   <si>
-    <t xml:space="preserve">19 %, 
+    <t xml:space="preserve">19 %
 5198</t>
   </si>
   <si>
@@ -433,37 +412,37 @@
     <t xml:space="preserve">Übersterblichkeit</t>
   </si>
   <si>
-    <t xml:space="preserve">-114.5 (-6,8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-183.25 (-10,7%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60,0%</t>
+    <t xml:space="preserve">-114 (-6,8%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-183 (-10,7%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60,5%</t>
   </si>
   <si>
     <t xml:space="preserve">-67 (-1,1%)</t>
   </si>
   <si>
-    <t xml:space="preserve">-131.5 ( -2,1%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">96,3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1217.5 (12,3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1658.5 ( 16,7%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36,2%</t>
+    <t xml:space="preserve">-132 ( -2,1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1218 (12,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1658 ( 16,7%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36,1%</t>
   </si>
   <si>
     <t xml:space="preserve">1036 ( 5,9%)</t>
   </si>
   <si>
-    <t xml:space="preserve">1343.75 (  7,5%)</t>
+    <t xml:space="preserve">1344 (  7,5%)</t>
   </si>
   <si>
     <t xml:space="preserve">29,7%</t>
@@ -596,7 +575,7 @@
     <t xml:space="preserve">Tschechien</t>
   </si>
   <si>
-    <t xml:space="preserve">6,6 %</t>
+    <t xml:space="preserve">5,4 %</t>
   </si>
   <si>
     <t xml:space="preserve">Italien</t>
@@ -614,7 +593,7 @@
     <t xml:space="preserve">Belgien</t>
   </si>
   <si>
-    <t xml:space="preserve">5,4 %</t>
+    <t xml:space="preserve">5,3 %</t>
   </si>
   <si>
     <t xml:space="preserve">Vereinigtes Königreich</t>
@@ -629,7 +608,7 @@
     <t xml:space="preserve">Frankreich</t>
   </si>
   <si>
-    <t xml:space="preserve">5,3 %</t>
+    <t xml:space="preserve">3,7 %</t>
   </si>
   <si>
     <t xml:space="preserve">3 %</t>
@@ -644,16 +623,13 @@
     <t xml:space="preserve">Spanien</t>
   </si>
   <si>
-    <t xml:space="preserve">4,6 %</t>
-  </si>
-  <si>
     <t xml:space="preserve">2,8 %</t>
   </si>
   <si>
     <t xml:space="preserve">12,2</t>
   </si>
   <si>
-    <t xml:space="preserve">4,3 %</t>
+    <t xml:space="preserve">3,6 %</t>
   </si>
   <si>
     <t xml:space="preserve">2,4 %</t>
@@ -662,25 +638,22 @@
     <t xml:space="preserve">11,3</t>
   </si>
   <si>
-    <t xml:space="preserve">4 %</t>
-  </si>
-  <si>
     <t xml:space="preserve">Deutschland</t>
   </si>
   <si>
     <t xml:space="preserve"> 8,8</t>
   </si>
   <si>
-    <t xml:space="preserve">3,7 %</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 8,6</t>
   </si>
   <si>
+    <t xml:space="preserve">2,9 %</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 6,9</t>
   </si>
   <si>
-    <t xml:space="preserve">3,6 %</t>
+    <t xml:space="preserve">2,7 %</t>
   </si>
   <si>
     <t xml:space="preserve"> 6,3</t>
@@ -1258,42 +1231,6 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" t="s">
-        <v>65</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1310,7 +1247,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1324,44 +1261,44 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1380,7 +1317,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1394,49 +1331,49 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
@@ -1444,47 +1381,47 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -1492,58 +1429,58 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D10" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D12" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1562,13 +1499,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1576,63 +1513,63 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B6"/>
       <c r="C6"/>
@@ -1640,58 +1577,58 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D8" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1710,7 +1647,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1724,13 +1661,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D2" t="n">
         <v>-5</v>
@@ -1738,13 +1675,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D3" t="n">
         <v>-2</v>
@@ -1752,13 +1689,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D4" t="n">
         <v>-15</v>
@@ -1780,24 +1717,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B2" t="n">
         <v>1.09</v>
@@ -1814,7 +1751,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B3" t="n">
         <v>1.14</v>
@@ -1831,7 +1768,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B4" t="n">
         <v>1.06</v>
@@ -1848,7 +1785,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B5" t="n">
         <v>1.06</v>
@@ -1865,7 +1802,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B6" t="n">
         <v>1.06</v>
@@ -1882,7 +1819,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -1899,7 +1836,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B8" t="n">
         <v>1.16</v>
@@ -1916,7 +1853,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B9" t="n">
         <v>1.08</v>
@@ -1933,7 +1870,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B10" t="n">
         <v>1.34</v>
@@ -1950,7 +1887,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B11" t="n">
         <v>1.03</v>
@@ -1967,7 +1904,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B12" t="n">
         <v>1.05</v>
@@ -1984,7 +1921,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B13" t="n">
         <v>1.08</v>
@@ -2001,7 +1938,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B14" t="n">
         <v>1.19</v>
@@ -2018,7 +1955,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B15" t="n">
         <v>1.12</v>
@@ -2035,7 +1972,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B16" t="n">
         <v>1.22</v>
@@ -2052,7 +1989,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B17" t="n">
         <v>1.21</v>
@@ -2069,7 +2006,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B18" t="n">
         <v>1.17</v>
@@ -2100,240 +2037,240 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" t="s">
         <v>178</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I1" t="s">
         <v>179</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J1" t="s">
         <v>180</v>
-      </c>
-      <c r="D1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F1" t="s">
-        <v>183</v>
-      </c>
-      <c r="G1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H1" t="s">
-        <v>185</v>
-      </c>
-      <c r="I1" t="s">
-        <v>186</v>
-      </c>
-      <c r="J1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C2" t="n">
-        <v>40755</v>
+        <v>579079</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="F2" t="n">
         <v>64520</v>
       </c>
       <c r="G2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="H2" t="n">
         <v>563</v>
       </c>
       <c r="I2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="J2" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C3" t="n">
-        <v>579079</v>
+        <v>608137</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E3" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="F3" t="n">
         <v>64267</v>
       </c>
       <c r="G3" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H3" t="n">
         <v>555</v>
       </c>
       <c r="I3" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="J3" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C4" t="n">
-        <v>608137</v>
+        <v>2432559</v>
       </c>
       <c r="D4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" t="s">
         <v>194</v>
-      </c>
-      <c r="E4" t="s">
-        <v>201</v>
       </c>
       <c r="F4" t="n">
         <v>17951</v>
       </c>
       <c r="G4" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="H4" t="n">
         <v>438</v>
       </c>
       <c r="I4" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="J4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="C5" t="n">
-        <v>96314</v>
+        <v>1730575</v>
       </c>
       <c r="D5" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="E5" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="F5" t="n">
         <v>47624</v>
       </c>
       <c r="G5" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="H5" t="n">
         <v>427</v>
       </c>
       <c r="I5" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="J5" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C6" t="n">
-        <v>175886</v>
+        <v>623567</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E6" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="F6" t="n">
         <v>13385</v>
       </c>
       <c r="G6" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="H6" t="n">
         <v>397</v>
       </c>
       <c r="I6" t="s">
+        <v>195</v>
+      </c>
+      <c r="J6" t="s">
         <v>202</v>
-      </c>
-      <c r="J6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="C7" t="n">
-        <v>1514</v>
+        <v>1843712</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E7" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="F7" t="n">
         <v>58015</v>
       </c>
       <c r="G7" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="H7" t="n">
         <v>353</v>
       </c>
       <c r="I7" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="J7" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="C8" t="n">
-        <v>2432559</v>
+        <v>1135676</v>
       </c>
       <c r="D8" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
@@ -2342,112 +2279,112 @@
         <v>22864</v>
       </c>
       <c r="G8" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="H8" t="n">
         <v>345</v>
       </c>
       <c r="I8" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="J8" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C9" t="n">
-        <v>1730575</v>
+        <v>556335</v>
       </c>
       <c r="D9" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F9" t="n">
         <v>9535</v>
       </c>
       <c r="G9" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="H9" t="n">
         <v>273</v>
       </c>
       <c r="I9" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="J9" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B10" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C10" t="n">
-        <v>623567</v>
+        <v>1854490</v>
       </c>
       <c r="D10" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F10" t="n">
         <v>22106</v>
       </c>
       <c r="G10" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="H10" t="n">
         <v>246</v>
       </c>
       <c r="I10" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="J10" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B11" t="s">
-        <v>217</v>
+        <v>81</v>
       </c>
       <c r="C11" t="n">
-        <v>322463</v>
+        <v>1350810</v>
       </c>
       <c r="D11" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F11" t="n">
         <v>10134</v>
       </c>
       <c r="G11" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="H11" t="n">
         <v>219</v>
       </c>
       <c r="I11" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="J11" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>